<commit_message>
Revise the visualisation of Bayesian network.
</commit_message>
<xml_diff>
--- a/docs/article_tables.xlsx
+++ b/docs/article_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sz_accidents\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\traffic-crash-characteristics-shenzhen\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7127C509-47C1-4877-8E95-018D0017B35F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D480965-EC19-42EE-B0AC-032C4609525C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4750" yWindow="1520" windowWidth="28800" windowHeight="15500" firstSheet="2" activeTab="2" xr2:uid="{E8498640-81FA-47AB-8FFE-956F719BE67B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="2" activeTab="9" xr2:uid="{E8498640-81FA-47AB-8FFE-956F719BE67B}"/>
   </bookViews>
   <sheets>
     <sheet name="Travel method" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="162">
   <si>
     <t>Age</t>
   </si>
@@ -1069,13 +1069,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F4CE05-5D86-40E9-93A5-869294BD98C0}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1653,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A532F852-0478-43C9-9189-17F13EA01DBE}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -4125,10 +4126,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F636C3F-64C0-438F-B4E5-08B8004C53FF}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4136,7 +4137,7 @@
     <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -4179,11 +4180,8 @@
       <c r="N1" t="s">
         <v>121</v>
       </c>
-      <c r="O1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -4226,12 +4224,8 @@
       <c r="N2" s="1">
         <v>11.041311614019699</v>
       </c>
-      <c r="O2" s="1">
-        <f>D3+F3+H3</f>
-        <v>63.8263186332047</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4274,210 +4268,143 @@
       <c r="N3" s="1">
         <v>3.9079239096007301</v>
       </c>
-      <c r="O3" s="1">
-        <f t="shared" ref="O3:O9" si="0">D4+F4+H4</f>
-        <v>33.111782477341357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10.1978046145785</v>
+      </c>
+      <c r="C4">
+        <v>16035</v>
+      </c>
+      <c r="D4" s="1">
+        <v>50.854714408042803</v>
+      </c>
+      <c r="E4">
+        <v>854</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.7084456566553499</v>
+      </c>
+      <c r="G4">
+        <v>1517</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4.8111382449018398</v>
+      </c>
+      <c r="I4">
+        <v>602</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.90923218419967</v>
+      </c>
+      <c r="K4">
+        <v>8673</v>
+      </c>
+      <c r="L4" s="1">
+        <v>27.5062636770162</v>
+      </c>
+      <c r="M4">
+        <v>3850</v>
+      </c>
+      <c r="N4" s="1">
+        <v>12.2102058291839</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.5084962838864904</v>
+      </c>
+      <c r="C5">
+        <v>1693</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12.144906743185</v>
+      </c>
+      <c r="E5">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.63845050215207999</v>
+      </c>
+      <c r="G5">
         <v>146</v>
       </c>
-      <c r="B4" s="1">
+      <c r="H5" s="1">
+        <v>1.0473457675753199</v>
+      </c>
+      <c r="I5">
+        <v>89</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.63845050215207999</v>
+      </c>
+      <c r="K5">
+        <v>10570</v>
+      </c>
+      <c r="L5" s="1">
+        <v>75.824964131994193</v>
+      </c>
+      <c r="M5">
+        <v>1353</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9.7058823529411704</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="1">
         <v>1.6057879519007401</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>790</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D6" s="1">
         <v>15.9113796576032</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>397</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F6" s="1">
         <v>7.9959718026183202</v>
       </c>
-      <c r="G4">
+      <c r="G6">
         <v>457</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H6" s="1">
         <v>9.2044310171198394</v>
       </c>
-      <c r="I4">
+      <c r="I6">
         <v>600</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J6" s="1">
         <v>12.084592145015099</v>
       </c>
-      <c r="K4">
+      <c r="K6">
         <v>1918</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L6" s="1">
         <v>38.630412890231597</v>
       </c>
-      <c r="M4">
+      <c r="M6">
         <v>803</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N6" s="1">
         <v>16.173212487411799</v>
       </c>
-      <c r="O4" s="1">
-        <f t="shared" si="0"/>
-        <v>58.374298309599993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="1">
-        <v>10.1978046145785</v>
-      </c>
-      <c r="C5">
-        <v>16035</v>
-      </c>
-      <c r="D5" s="1">
-        <v>50.854714408042803</v>
-      </c>
-      <c r="E5">
-        <v>854</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.7084456566553499</v>
-      </c>
-      <c r="G5">
-        <v>1517</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4.8111382449018398</v>
-      </c>
-      <c r="I5">
-        <v>602</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1.90923218419967</v>
-      </c>
-      <c r="K5">
-        <v>8673</v>
-      </c>
-      <c r="L5" s="1">
-        <v>27.5062636770162</v>
-      </c>
-      <c r="M5">
-        <v>3850</v>
-      </c>
-      <c r="N5" s="1">
-        <v>12.2102058291839</v>
-      </c>
-      <c r="O5" s="1">
-        <f t="shared" si="0"/>
-        <v>13.830703012912402</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4.5084962838864904</v>
-      </c>
-      <c r="C6">
-        <v>1693</v>
-      </c>
-      <c r="D6" s="1">
-        <v>12.144906743185</v>
-      </c>
-      <c r="E6">
-        <v>89</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.63845050215207999</v>
-      </c>
-      <c r="G6">
-        <v>146</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1.0473457675753199</v>
-      </c>
-      <c r="I6">
-        <v>89</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.63845050215207999</v>
-      </c>
-      <c r="K6">
-        <v>10570</v>
-      </c>
-      <c r="L6" s="1">
-        <v>75.824964131994193</v>
-      </c>
-      <c r="M6">
-        <v>1353</v>
-      </c>
-      <c r="N6" s="1">
-        <v>9.7058823529411704</v>
-      </c>
-      <c r="O6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.14531253547669312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>10.092068962356599</v>
-      </c>
-      <c r="C7">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.9902368140226502E-2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.27050836682333E-3</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1">
-        <v>4.3139658969643301E-2</v>
-      </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1.8164066934586599E-2</v>
-      </c>
-      <c r="K7">
-        <v>166</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0.37690438889267303</v>
-      </c>
-      <c r="M7">
-        <v>43805</v>
-      </c>
-      <c r="N7" s="1">
-        <v>99.459619008695995</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O9" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N6">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>